<commit_message>
player data scrapping complete, with the correct number of players
</commit_message>
<xml_diff>
--- a/scraped_nba_data.xlsx
+++ b/scraped_nba_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="167">
   <si>
     <t>Player</t>
   </si>
@@ -139,12 +139,18 @@
     <t>Max Christie</t>
   </si>
   <si>
+    <t>Gabriele Procida</t>
+  </si>
+  <si>
     <t>Jaden Hardy</t>
   </si>
   <si>
     <t>Kennedy Chandler</t>
   </si>
   <si>
+    <t>Khalifa Diop</t>
+  </si>
+  <si>
     <t>Bryce McGowens</t>
   </si>
   <si>
@@ -163,6 +169,9 @@
     <t>Josh Minott</t>
   </si>
   <si>
+    <t>Ismael Kamagate</t>
+  </si>
+  <si>
     <t>Vince Williams Jr.</t>
   </si>
   <si>
@@ -172,6 +181,9 @@
     <t>Isaiah Mobley</t>
   </si>
   <si>
+    <t>Matteo Spagnolo</t>
+  </si>
+  <si>
     <t>Orlando Magic</t>
   </si>
   <si>
@@ -346,6 +358,15 @@
     <t>Paris (France)</t>
   </si>
   <si>
+    <t>Virginia Commonwealth</t>
+  </si>
+  <si>
+    <t>Southern California</t>
+  </si>
+  <si>
+    <t>Vanoli Cremona (Italy)</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -482,6 +503,18 @@
   </si>
   <si>
     <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
   </si>
 </sst>
 </file>
@@ -839,7 +872,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -870,19 +903,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -890,19 +923,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -910,19 +943,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -930,19 +963,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -950,19 +983,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -970,19 +1003,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="F7" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -990,19 +1023,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1010,19 +1043,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F9" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1030,19 +1063,19 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1050,19 +1083,19 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E11" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F11" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1070,19 +1103,19 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="F12" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1090,19 +1123,19 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E13" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1110,19 +1143,19 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1130,19 +1163,19 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E15" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1150,19 +1183,19 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E16" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="F16" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1170,19 +1203,19 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1190,19 +1223,19 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E18" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1210,19 +1243,19 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E19" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F19" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1230,19 +1263,19 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E20" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1250,19 +1283,19 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1270,19 +1303,19 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F22" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1290,19 +1323,19 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E23" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="F23" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1310,19 +1343,19 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D24" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E24" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="F24" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1330,19 +1363,19 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E25" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="F25" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1350,19 +1383,19 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E26" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="F26" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1370,19 +1403,19 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E27" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="F27" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1390,19 +1423,19 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D28" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E28" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="F28" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1410,19 +1443,19 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E29" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="F29" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1430,19 +1463,19 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E30" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="F30" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1450,19 +1483,19 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D31" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="E31" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="F31" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1470,19 +1503,19 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="F32" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1490,19 +1523,19 @@
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E33" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F33" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1510,19 +1543,19 @@
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E34" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="F34" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1530,19 +1563,19 @@
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D35" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E35" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="F35" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1550,19 +1583,19 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E36" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="F36" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1570,19 +1603,19 @@
         <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E37" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="F37" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1590,19 +1623,19 @@
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E38" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="F38" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1610,19 +1643,19 @@
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D39" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E39" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F39" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1630,19 +1663,19 @@
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D40" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E40" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="F40" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1650,19 +1683,19 @@
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D41" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E41" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F41" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1670,19 +1703,19 @@
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E42" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="F42" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1690,19 +1723,19 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E43" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="F43" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1710,19 +1743,19 @@
         <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E44" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="F44" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1730,19 +1763,19 @@
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D45" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E45" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="F45" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1750,19 +1783,19 @@
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D46" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E46" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="F46" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1770,19 +1803,99 @@
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D47" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E47" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F47" t="s">
-        <v>155</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" t="s">
+        <v>133</v>
+      </c>
+      <c r="F48" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" t="s">
+        <v>134</v>
+      </c>
+      <c r="F49" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E50" t="s">
+        <v>135</v>
+      </c>
+      <c r="F50" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" t="s">
+        <v>116</v>
+      </c>
+      <c r="D51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E51" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>